<commit_message>
trinity add run method and log utils
</commit_message>
<xml_diff>
--- a/example/excel_trinity/score.xlsx
+++ b/example/excel_trinity/score.xlsx
@@ -1648,7 +1648,7 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D7">
         <v>92</v>
@@ -1665,10 +1665,12 @@
       <c r="H7">
         <v>94</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="str">
+        <f>=SUM(C7:H7)</f>
         <v>548</v>
       </c>
-      <c r="J7">
+      <c r="J7" t="str">
+        <f>=AVERAGE(C7:H7)</f>
         <v>91.33</v>
       </c>
     </row>

</xml_diff>